<commit_message>
Arbeitsnachweis einbinden und Diplseminar beginnen
</commit_message>
<xml_diff>
--- a/form/Arbeitsnachweis.xlsx
+++ b/form/Arbeitsnachweis.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17766"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="229">
   <si>
     <t>Arbeit</t>
   </si>
@@ -550,54 +550,21 @@
     <t>Recherche zum Gesamtprojekt (Verstärker, Weichen, Bluetooth) (5h)</t>
   </si>
   <si>
-    <t>TTVerstärker PCB neu überlegt (v2) (5h), HT/TTVerstärker PCB überarbeitet (8h)</t>
-  </si>
-  <si>
-    <t>Vorbereitung der Mess-Lautsprecher-Chassis (4h), TTVerstärker PCB v1 layouten (2h), HTVerstärker PCB v1 layouten (3h), HTVerstärker&amp;TTVerstärker PCB v1 anpassen (1h)</t>
-  </si>
-  <si>
     <t>mTT-Weiche+Addiererschaltung PCB &amp; Schematic erstellen (3h)</t>
   </si>
   <si>
-    <t>mTT-Weiche+Addiererschaltung PCB überarbeiten (1h), HTuTTWeiche PCB+Schematic erstellen (2h)</t>
-  </si>
-  <si>
-    <t>Bauteilbeschaffung für Verstärkerprints (1h), Bestücken der Verstärkerprints (2h), Frequenzweichen finalisiert und in Auftrag gegeben(1h), Korregieren der Verstärkerprints(1h)</t>
-  </si>
-  <si>
-    <t>Tieftöner Hochtöner und Subwoofer Messungen (9h)</t>
-  </si>
-  <si>
     <t>Lautsprechermessung (4h), Kühlkörper für Verstärkerprints bearbeitet (5h)</t>
   </si>
   <si>
-    <t xml:space="preserve"> Kühlkörper für Verstärkerprints bearbeitet (3h), Verstärkerprints testen, messen, bearbeiten (2h), </t>
-  </si>
-  <si>
     <t>Lautsprechermessungen (5h), Auswertung der Messungen (1h), Weichenprints anpassen (4h)</t>
   </si>
   <si>
     <t>Lautsprecher messen (Subwoofer mit Styropor und Ytong-Ziegel) (4h), Schaltung HTuTT-Weiche optimieren (5h)</t>
   </si>
   <si>
-    <t>Projekt-Files anpassen und FabricationOutputs generieren (2,5h), 3_mTTWeiche+Addierschaltung für Printerei vorbereiten (0,5h), 2_Hauptboard bearbeiten (0,5h), einstellbares Filter testen (1h), Kontrollmessungen mit Filter (1h), Lautsprechermessungen (5,5h), Prints 2,3 und 4 verbessern (2h)</t>
-  </si>
-  <si>
-    <t>Testen des Messequipments (1h), Lautsprechermessungen: 2-Weg-System(TT1+AE1004) mit Stereo-Verstärker aufgebaut und mit Filter angepasst (5h)</t>
-  </si>
-  <si>
-    <t>Brüel&amp;Kjaer 2 Messungen in ein Diagram (2h), Recherche (HT, Ladegerät) (1,5h),  Printbohrungen erweitern(0,5h), Überlegungen zur Subwooferbox (1h)</t>
-  </si>
-  <si>
-    <t>Messungen DTW 72-8 &amp; + TT1 (2h), Entwurf von Elektronikschacht in der Subwooferbox (2h)</t>
-  </si>
-  <si>
     <t>Dokumentation (15h)</t>
   </si>
   <si>
-    <t>Subwooferverstärker testen (5h), TT- und HT-Verstärker testen (1h), Frontplatine testen (2h), Netzteilüberelegungen (1h)</t>
-  </si>
-  <si>
     <t>TT- und HT-Verstärker testen &amp; verbessern (5h), Frontplatine mit Hauptplatine testen &amp; verbessern (3h), über Netzteile informieren (1h)</t>
   </si>
   <si>
@@ -619,12 +586,6 @@
     <t>Gesamt Stundenzahl:</t>
   </si>
   <si>
-    <t>Recherche zum Gesamtprojekt (10h), Erstellen eines Blockschaltbilds und Überarbeiten (6h)</t>
-  </si>
-  <si>
-    <t>Gehäuseberechnungen - Mono-Subwooferbox und Satelliten-Boxen (1h),  Thiele Small Parameter einlesen (1h), Analoge Verstärker Schaltung (Recherche &amp; Bauteilbestandsaufnahme) (1h), Altium Libarys für Entwicklung bestimmen und einbinden (1h)</t>
-  </si>
-  <si>
     <t>Analog-Verstärker (Recherche und Schaltung zeichnen) (5h), Recherche - geeignete Leistungs-Transistoren (1h), Zeitplan für die Diplomarbeit (1h)</t>
   </si>
   <si>
@@ -679,9 +640,6 @@
     <t>Lautsprecher messen (Subwoofer mit Styropor und Ytong-Ziegel) (4h), Ergebnisse interpretieren (1h), Weichen optimieren (4h)</t>
   </si>
   <si>
-    <t>Testen des Messequpments (1h), Lautsprechermessungen mit stark verkleinertem Volumen und Filter (7h)</t>
-  </si>
-  <si>
     <t>Lautsprechermessungen: 2-Weg-System(TT1+AE1004) mit Stereo-Verstärker aufgebaut und mit Filter angepasst (5h)</t>
   </si>
   <si>
@@ -716,6 +674,42 @@
   </si>
   <si>
     <t>Dokumentation (5h)</t>
+  </si>
+  <si>
+    <t>Recherche zum Gesamtprojekt (10h), Entwurf eines Blockschaltbilds und Überarbeiten (6h)</t>
+  </si>
+  <si>
+    <t>Gehäuseberechnungen - Subwooferbox und Satelliten-Boxen (1h),  TSP einlesen (1h), Analog-Verstärker (Recherche &amp; Bauteilbestandsaufnahme) (1h), Altium einrichten (1h)</t>
+  </si>
+  <si>
+    <t>Vorbereitung der Lautsprecher-Chassis für Messungen (4h), TTVerstärker PCB layouten (2h), HTVerstärker PCB layouten (3h), HTVerstärker &amp; TTVerstärker PCB anpassen (1h)</t>
+  </si>
+  <si>
+    <t>TTVerstärker PCB neu überlegt (5h), HT-/TTVerstärker PCB überarbeitet (8h)</t>
+  </si>
+  <si>
+    <t>mTT-Weiche+Addiererschaltung PCB überarbeiten (1h), HTuTTWeiche PCB &amp; Schematic erstellen (2h)</t>
+  </si>
+  <si>
+    <t>Bauteilbeschaffung für Verstärkerprints (1h), Bestücken der Verstärkerprints (2h), Frequenzweichen finalisiert (1h), Korregieren der Verstärkerprints(1h)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kühlkörper für Verstärkerprints bearbeitet (3h), Verstärkerprints testen, messen, bearbeiten (2h), </t>
+  </si>
+  <si>
+    <t>Testen des Messequipments (1h), Lautsprechermessungen mit stark verkleinertem Volumen und Filter (7h)</t>
+  </si>
+  <si>
+    <t>Projekt-Files anpassen (2,5h),  Hauptboard bearbeiten (1h), einstellbares Filter testen (1h), Lautsprechermessungen (6,5h), Testen des Messequipments (1h), Prints 2,3 und 4 verbessern (2h)</t>
+  </si>
+  <si>
+    <t>Brüel&amp;Kjaer 2 Messungen in ein Diagram (2h), Recherche (HT &amp; Ladegerät) (1,5h),  Printbohrungen erweitern(0,5h), Überlegungen zur Subwooferbox (1h)</t>
+  </si>
+  <si>
+    <t>Messungen DTW 72-8 &amp; TT1 (2h), Entwurf von Elektronikschacht in der Subwooferbox (2h)</t>
+  </si>
+  <si>
+    <t>Subwoofer-Verstärker testen (5h), TT- und HT-Verstärker testen (1h), Frontplatine testen (2h), Netzteilüberelegungen (1h)</t>
   </si>
 </sst>
 </file>
@@ -771,7 +765,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -868,11 +862,182 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -956,18 +1121,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -975,6 +1128,18 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
@@ -985,6 +1150,51 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1306,22 +1516,22 @@
       <selection activeCell="D64" sqref="D64"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="15.88671875" customWidth="1"/>
-    <col min="3" max="3" width="37.6640625" customWidth="1"/>
-    <col min="4" max="4" width="10.5546875" style="5" customWidth="1"/>
-    <col min="5" max="5" width="15.44140625" customWidth="1"/>
-    <col min="7" max="7" width="15.44140625" customWidth="1"/>
-    <col min="8" max="8" width="37.6640625" customWidth="1"/>
-    <col min="9" max="9" width="6.5546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.44140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="20.44140625" customWidth="1"/>
-    <col min="14" max="14" width="17.88671875" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" customWidth="1"/>
+    <col min="3" max="3" width="37.7109375" customWidth="1"/>
+    <col min="4" max="4" width="10.5703125" style="5" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" customWidth="1"/>
+    <col min="7" max="7" width="15.42578125" customWidth="1"/>
+    <col min="8" max="8" width="37.7109375" customWidth="1"/>
+    <col min="9" max="9" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20.42578125" customWidth="1"/>
+    <col min="14" max="14" width="17.85546875" customWidth="1"/>
     <col min="15" max="15" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B2" s="9" t="s">
         <v>10</v>
       </c>
@@ -1353,7 +1563,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:16" x14ac:dyDescent="0.25">
       <c r="I3" s="5"/>
       <c r="M3" t="s">
         <v>6</v>
@@ -1366,7 +1576,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>1</v>
       </c>
@@ -1399,7 +1609,7 @@
         <v>45.940000000000005</v>
       </c>
     </row>
-    <row r="5" spans="2:16" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:16" ht="45" x14ac:dyDescent="0.25">
       <c r="B5" s="14">
         <v>42597</v>
       </c>
@@ -1428,7 +1638,7 @@
         <v>57.48</v>
       </c>
     </row>
-    <row r="6" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B6" s="14">
         <v>42619</v>
       </c>
@@ -1457,7 +1667,7 @@
         <v>34.729999999999997</v>
       </c>
     </row>
-    <row r="7" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B7" s="14">
         <v>42620</v>
       </c>
@@ -1486,7 +1696,7 @@
         <v>9.24</v>
       </c>
     </row>
-    <row r="8" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B8" s="14">
         <v>42621</v>
       </c>
@@ -1515,7 +1725,7 @@
         <v>10.14</v>
       </c>
     </row>
-    <row r="9" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B9" s="14">
         <v>42622</v>
       </c>
@@ -1542,7 +1752,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="2:16" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:16" ht="30" x14ac:dyDescent="0.25">
       <c r="B10" s="14">
         <v>42634</v>
       </c>
@@ -1562,7 +1772,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="2:16" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:16" ht="45" x14ac:dyDescent="0.25">
       <c r="B11" s="14">
         <v>42641</v>
       </c>
@@ -1580,7 +1790,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B12" s="14"/>
       <c r="C12" t="s">
         <v>13</v>
@@ -1598,7 +1808,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B13" s="14">
         <v>42647</v>
       </c>
@@ -1615,7 +1825,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B14" s="14">
         <v>42648</v>
       </c>
@@ -1635,7 +1845,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B15" s="14">
         <v>42655</v>
       </c>
@@ -1655,7 +1865,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B16" s="14">
         <v>42656</v>
       </c>
@@ -1673,7 +1883,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="17" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:9" ht="45" x14ac:dyDescent="0.25">
       <c r="B17" s="14">
         <v>42662</v>
       </c>
@@ -1693,7 +1903,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B18" s="14">
         <v>42669</v>
       </c>
@@ -1711,7 +1921,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B19" s="14">
         <v>42670</v>
       </c>
@@ -1731,7 +1941,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B20" s="14">
         <v>42676</v>
       </c>
@@ -1751,7 +1961,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B21" s="14" t="s">
         <v>37</v>
       </c>
@@ -1771,7 +1981,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="22" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B22" s="14"/>
       <c r="C22" s="11" t="s">
         <v>39</v>
@@ -1789,7 +1999,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="23" spans="2:9" ht="72" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:9" ht="75" x14ac:dyDescent="0.25">
       <c r="B23" s="14"/>
       <c r="C23" s="11" t="s">
         <v>40</v>
@@ -1805,7 +2015,7 @@
         <v>2.25</v>
       </c>
     </row>
-    <row r="24" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B24" s="14" t="s">
         <v>44</v>
       </c>
@@ -1825,7 +2035,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B25" s="14" t="s">
         <v>51</v>
       </c>
@@ -1843,7 +2053,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B26" s="14">
         <v>42711</v>
       </c>
@@ -1861,7 +2071,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C27" t="s">
         <v>54</v>
       </c>
@@ -1876,7 +2086,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:9" ht="30" x14ac:dyDescent="0.25">
       <c r="C28" t="s">
         <v>55</v>
       </c>
@@ -1893,7 +2103,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B29" s="14" t="s">
         <v>52</v>
       </c>
@@ -1913,7 +2123,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:9" ht="30" x14ac:dyDescent="0.25">
       <c r="C30" t="s">
         <v>57</v>
       </c>
@@ -1928,7 +2138,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B31" s="14" t="s">
         <v>59</v>
       </c>
@@ -1948,7 +2158,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B32" s="14"/>
       <c r="C32" t="s">
         <v>62</v>
@@ -1964,7 +2174,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B33" s="14"/>
       <c r="C33" t="s">
         <v>61</v>
@@ -1982,7 +2192,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="2:9" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:9" ht="45" x14ac:dyDescent="0.25">
       <c r="B34" s="14">
         <v>42742</v>
       </c>
@@ -2000,7 +2210,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B35" s="14"/>
       <c r="C35" t="s">
         <v>72</v>
@@ -2016,7 +2226,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="36" spans="2:9" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:9" ht="60" x14ac:dyDescent="0.25">
       <c r="B36" s="16">
         <v>42746</v>
       </c>
@@ -2036,7 +2246,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="37" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B37" s="14">
         <v>42753</v>
       </c>
@@ -2054,7 +2264,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="38" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B38" s="14"/>
       <c r="C38" t="s">
         <v>82</v>
@@ -2072,7 +2282,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="39" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B39" s="14"/>
       <c r="C39" s="11" t="s">
         <v>83</v>
@@ -2088,7 +2298,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B40" s="14"/>
       <c r="C40" t="s">
         <v>84</v>
@@ -2106,7 +2316,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B41" s="14">
         <v>42760</v>
       </c>
@@ -2126,7 +2336,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B42" s="14">
         <v>42767</v>
       </c>
@@ -2144,7 +2354,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B43" s="14"/>
       <c r="C43" s="11" t="s">
         <v>87</v>
@@ -2160,7 +2370,7 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="44" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B44" s="14">
         <v>42774</v>
       </c>
@@ -2180,7 +2390,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="45" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B45" s="14">
         <v>42776</v>
       </c>
@@ -2200,7 +2410,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="2:9" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:9" ht="60" x14ac:dyDescent="0.25">
       <c r="B46" s="14">
         <v>42777</v>
       </c>
@@ -2218,7 +2428,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="47" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B47" s="14" t="s">
         <v>96</v>
       </c>
@@ -2238,7 +2448,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="48" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B48" s="14"/>
       <c r="C48" t="s">
         <v>98</v>
@@ -2254,7 +2464,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="49" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B49" s="14"/>
       <c r="C49" t="s">
         <v>99</v>
@@ -2270,7 +2480,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B50" s="14"/>
       <c r="C50" t="s">
         <v>100</v>
@@ -2286,7 +2496,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="51" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B51" s="14" t="s">
         <v>106</v>
       </c>
@@ -2304,7 +2514,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B52" s="14"/>
       <c r="C52" s="11" t="s">
         <v>108</v>
@@ -2322,7 +2532,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="53" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B53" s="14"/>
       <c r="C53" t="s">
         <v>109</v>
@@ -2338,7 +2548,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="54" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B54" s="14">
         <v>42738</v>
       </c>
@@ -2358,7 +2568,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="55" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B55" s="14"/>
       <c r="C55" t="s">
         <v>112</v>
@@ -2376,7 +2586,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="56" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B56" s="14"/>
       <c r="C56" t="s">
         <v>113</v>
@@ -2392,7 +2602,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="57" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:9" ht="45" x14ac:dyDescent="0.25">
       <c r="B57" s="14"/>
       <c r="C57" t="s">
         <v>114</v>
@@ -2410,7 +2620,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="58" spans="2:9" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="58" spans="2:9" ht="60" x14ac:dyDescent="0.25">
       <c r="B58" s="14">
         <v>42802</v>
       </c>
@@ -2428,7 +2638,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="59" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="59" spans="2:9" ht="45" x14ac:dyDescent="0.25">
       <c r="B59" s="14"/>
       <c r="C59" s="11" t="s">
         <v>123</v>
@@ -2446,7 +2656,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="60" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="60" spans="2:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B60" s="14">
         <v>42805</v>
       </c>
@@ -2466,7 +2676,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="61" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="61" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B61" s="14">
         <v>42806</v>
       </c>
@@ -2484,7 +2694,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="62" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B62" s="14">
         <v>42807</v>
       </c>
@@ -2502,7 +2712,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="63" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="63" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B63" s="14"/>
       <c r="D63" s="10"/>
       <c r="G63" s="18"/>
@@ -2513,7 +2723,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="64" spans="2:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B64" s="14"/>
       <c r="D64" s="10"/>
       <c r="G64" s="20">
@@ -2526,7 +2736,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="65" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="65" spans="2:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B65" s="14"/>
       <c r="D65" s="10"/>
       <c r="H65" s="11" t="s">
@@ -2536,7 +2746,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="66" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="66" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B66" s="14"/>
       <c r="D66" s="10"/>
       <c r="H66" t="s">
@@ -2546,7 +2756,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="67" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B67" s="14"/>
       <c r="D67" s="10"/>
       <c r="H67" t="s">
@@ -2556,7 +2766,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="68" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B68" s="14"/>
       <c r="D68" s="10"/>
       <c r="G68" s="20">
@@ -2569,7 +2779,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="69" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="69" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B69" s="14"/>
       <c r="D69" s="10"/>
       <c r="H69" t="s">
@@ -2579,7 +2789,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="70" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="70" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B70" s="14"/>
       <c r="D70" s="10"/>
       <c r="H70" t="s">
@@ -2589,7 +2799,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="71" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="71" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B71" s="14"/>
       <c r="D71" s="10"/>
       <c r="G71" s="20">
@@ -2602,7 +2812,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="72" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="72" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B72" s="1"/>
       <c r="D72" s="10"/>
       <c r="H72" t="s">
@@ -2612,7 +2822,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="73" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B73" s="1"/>
       <c r="D73" s="10"/>
       <c r="G73" s="20">
@@ -2625,7 +2835,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="74" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B74" s="1"/>
       <c r="D74" s="10"/>
       <c r="G74" s="20">
@@ -2638,7 +2848,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="75" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="75" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B75" s="1"/>
       <c r="D75" s="10"/>
       <c r="H75" t="s">
@@ -2648,7 +2858,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="76" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="76" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B76" s="1"/>
       <c r="D76" s="10"/>
       <c r="H76" t="s">
@@ -2658,7 +2868,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="77" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B77" s="1"/>
       <c r="D77" s="10"/>
       <c r="H77" t="s">
@@ -2668,7 +2878,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="78" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="78" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B78" s="1"/>
       <c r="D78" s="10"/>
       <c r="H78" t="s">
@@ -2678,7 +2888,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="79" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B79" s="1"/>
       <c r="D79" s="10"/>
       <c r="G79" s="20">
@@ -2691,13 +2901,13 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="80" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="80" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B80" s="1"/>
       <c r="D80" s="10"/>
       <c r="H80" s="37"/>
       <c r="I80" s="38"/>
     </row>
-    <row r="81" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="81" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B81" s="1"/>
       <c r="D81" s="10"/>
       <c r="G81" s="20">
@@ -2710,7 +2920,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="82" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="82" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B82" s="1"/>
       <c r="D82" s="10"/>
       <c r="G82" s="20">
@@ -2723,7 +2933,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="83" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="83" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B83" s="1"/>
       <c r="D83" s="10"/>
       <c r="G83" s="20">
@@ -2736,7 +2946,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="84" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="84" spans="2:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B84" s="1"/>
       <c r="D84" s="10"/>
       <c r="G84" s="20">
@@ -2749,7 +2959,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="85" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="85" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B85" s="1"/>
       <c r="D85" s="10"/>
       <c r="H85" t="s">
@@ -2759,7 +2969,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="86" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="86" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B86" s="1"/>
       <c r="D86" s="10"/>
       <c r="G86" s="20">
@@ -2772,7 +2982,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="87" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="87" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B87" s="1"/>
       <c r="D87" s="10"/>
       <c r="H87" t="s">
@@ -2782,7 +2992,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="88" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="88" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B88" s="1"/>
       <c r="D88" s="10"/>
       <c r="H88" t="s">
@@ -2792,7 +3002,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="89" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="89" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B89" s="1"/>
       <c r="D89" s="10"/>
       <c r="H89" t="s">
@@ -2802,7 +3012,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="90" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="90" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B90" s="1"/>
       <c r="D90" s="10"/>
       <c r="G90" s="20">
@@ -2815,7 +3025,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="91" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="91" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B91" s="1"/>
       <c r="D91" s="10"/>
       <c r="G91" s="20">
@@ -2828,7 +3038,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="92" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="92" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B92" s="1"/>
       <c r="D92" s="10"/>
       <c r="H92" t="s">
@@ -2838,7 +3048,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="93" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B93" s="1"/>
       <c r="D93" s="10"/>
       <c r="G93" s="20">
@@ -2851,7 +3061,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="94" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="94" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B94" s="1"/>
       <c r="D94" s="10"/>
       <c r="H94" t="s">
@@ -2861,7 +3071,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="95" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="95" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B95" s="1"/>
       <c r="D95" s="10"/>
       <c r="G95" s="20">
@@ -2874,7 +3084,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="96" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="96" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B96" s="1"/>
       <c r="D96" s="10"/>
       <c r="G96" s="20">
@@ -2887,180 +3097,180 @@
         <v>2</v>
       </c>
     </row>
-    <row r="97" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="97" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B97" s="1"/>
       <c r="D97" s="10"/>
     </row>
-    <row r="98" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="98" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B98" s="1"/>
       <c r="D98" s="10"/>
     </row>
-    <row r="99" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="99" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B99" s="1"/>
       <c r="D99" s="10"/>
     </row>
-    <row r="100" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="100" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B100" s="1"/>
       <c r="D100" s="10"/>
     </row>
-    <row r="101" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="101" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B101" s="1"/>
       <c r="D101" s="10"/>
     </row>
-    <row r="102" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="102" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B102" s="1"/>
       <c r="D102" s="10"/>
     </row>
-    <row r="103" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="103" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B103" s="1"/>
       <c r="D103" s="10"/>
     </row>
-    <row r="104" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="104" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B104" s="1"/>
       <c r="D104" s="10"/>
     </row>
-    <row r="105" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="105" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B105" s="1"/>
       <c r="D105" s="10"/>
     </row>
-    <row r="106" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="106" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B106" s="1"/>
       <c r="D106" s="10"/>
     </row>
-    <row r="107" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="107" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B107" s="1"/>
       <c r="D107" s="10"/>
     </row>
-    <row r="108" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="108" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B108" s="1"/>
       <c r="D108" s="10"/>
     </row>
-    <row r="109" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="109" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B109" s="1"/>
       <c r="D109" s="10"/>
     </row>
-    <row r="110" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="110" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B110" s="1"/>
       <c r="D110" s="10"/>
     </row>
-    <row r="111" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="111" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B111" s="1"/>
       <c r="D111" s="10"/>
     </row>
-    <row r="112" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="112" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B112" s="1"/>
       <c r="D112" s="10"/>
     </row>
-    <row r="113" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="113" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B113" s="1"/>
       <c r="D113" s="10"/>
     </row>
-    <row r="114" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="114" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B114" s="1"/>
       <c r="D114" s="10"/>
     </row>
-    <row r="115" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="115" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B115" s="1"/>
       <c r="D115" s="10"/>
     </row>
-    <row r="116" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="116" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B116" s="1"/>
       <c r="D116" s="10"/>
     </row>
-    <row r="117" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="117" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B117" s="1"/>
       <c r="D117" s="10"/>
     </row>
-    <row r="118" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="118" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B118" s="1"/>
       <c r="D118" s="10"/>
     </row>
-    <row r="119" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="119" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B119" s="1"/>
       <c r="D119" s="10"/>
     </row>
-    <row r="120" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="120" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B120" s="1"/>
       <c r="D120" s="10"/>
     </row>
-    <row r="121" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="121" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B121" s="1"/>
       <c r="D121" s="10"/>
     </row>
-    <row r="122" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="122" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B122" s="1"/>
       <c r="D122" s="10"/>
     </row>
-    <row r="123" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="123" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B123" s="1"/>
       <c r="D123" s="10"/>
     </row>
-    <row r="124" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="124" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B124" s="1"/>
       <c r="D124" s="10"/>
     </row>
-    <row r="125" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="125" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B125" s="1"/>
       <c r="D125" s="10"/>
     </row>
-    <row r="126" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="126" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B126" s="1"/>
       <c r="D126" s="10"/>
     </row>
-    <row r="127" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="127" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B127" s="1"/>
       <c r="D127" s="10"/>
     </row>
-    <row r="128" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="128" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B128" s="1"/>
       <c r="D128" s="10"/>
     </row>
-    <row r="129" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="129" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B129" s="1"/>
       <c r="D129" s="10"/>
     </row>
-    <row r="130" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="130" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B130" s="1"/>
       <c r="D130" s="10"/>
     </row>
-    <row r="131" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="131" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B131" s="1"/>
       <c r="D131" s="10"/>
     </row>
-    <row r="132" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="132" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B132" s="1"/>
       <c r="D132" s="10"/>
     </row>
-    <row r="133" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="133" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B133" s="1"/>
       <c r="D133" s="10"/>
     </row>
-    <row r="134" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="134" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B134" s="1"/>
       <c r="D134" s="10"/>
     </row>
-    <row r="135" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="135" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B135" s="1"/>
       <c r="D135" s="10"/>
     </row>
-    <row r="136" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="136" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B136" s="1"/>
       <c r="D136" s="10"/>
     </row>
-    <row r="137" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="137" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B137" s="1"/>
       <c r="D137" s="10"/>
     </row>
-    <row r="138" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="138" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B138" s="1"/>
     </row>
-    <row r="139" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="139" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B139" s="1"/>
     </row>
-    <row r="140" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="140" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B140" s="1"/>
     </row>
-    <row r="141" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="141" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B141" s="1"/>
     </row>
   </sheetData>
@@ -3079,786 +3289,761 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J87"/>
   <sheetViews>
-    <sheetView showGridLines="0" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29:F29"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageLayout" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23:F23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.109375" customWidth="1"/>
+    <col min="1" max="1" width="14.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="43" t="s">
-        <v>201</v>
-      </c>
-      <c r="B1" s="43" t="s">
+    <row r="1" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="52" t="s">
+        <v>188</v>
+      </c>
+      <c r="B1" s="54" t="s">
         <v>146</v>
       </c>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
-      <c r="G1" s="43" t="s">
+      <c r="C1" s="55"/>
+      <c r="D1" s="55"/>
+      <c r="E1" s="55"/>
+      <c r="F1" s="56"/>
+      <c r="G1" s="52" t="s">
         <v>147</v>
       </c>
       <c r="H1" s="1"/>
     </row>
-    <row r="2" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="44"/>
-      <c r="B2" s="44"/>
-      <c r="C2" s="44"/>
-      <c r="D2" s="44"/>
-      <c r="E2" s="44"/>
-      <c r="F2" s="44"/>
-      <c r="G2" s="44"/>
+    <row r="2" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="53"/>
+      <c r="B2" s="57"/>
+      <c r="C2" s="58"/>
+      <c r="D2" s="58"/>
+      <c r="E2" s="58"/>
+      <c r="F2" s="59"/>
+      <c r="G2" s="53"/>
       <c r="H2" s="1"/>
     </row>
-    <row r="3" spans="1:8" ht="56.55" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="56.65" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="31" t="s">
         <v>173</v>
       </c>
-      <c r="B3" s="45" t="s">
+      <c r="B3" s="49" t="s">
         <v>174</v>
       </c>
-      <c r="C3" s="45"/>
-      <c r="D3" s="45"/>
-      <c r="E3" s="45"/>
-      <c r="F3" s="45"/>
+      <c r="C3" s="50"/>
+      <c r="D3" s="50"/>
+      <c r="E3" s="50"/>
+      <c r="F3" s="51"/>
       <c r="G3" s="32">
         <v>5</v>
       </c>
       <c r="H3" s="1"/>
     </row>
-    <row r="4" spans="1:8" ht="56.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="56.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="29" t="s">
         <v>148</v>
       </c>
-      <c r="B4" s="41" t="s">
-        <v>198</v>
-      </c>
-      <c r="C4" s="41"/>
-      <c r="D4" s="41"/>
-      <c r="E4" s="41"/>
-      <c r="F4" s="41"/>
+      <c r="B4" s="46" t="s">
+        <v>217</v>
+      </c>
+      <c r="C4" s="47"/>
+      <c r="D4" s="47"/>
+      <c r="E4" s="47"/>
+      <c r="F4" s="48"/>
       <c r="G4" s="30">
         <v>16</v>
       </c>
       <c r="H4" s="1"/>
     </row>
-    <row r="5" spans="1:8" ht="56.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" ht="56.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="29" t="s">
         <v>149</v>
       </c>
-      <c r="B5" s="41" t="s">
-        <v>199</v>
-      </c>
-      <c r="C5" s="41"/>
-      <c r="D5" s="41"/>
-      <c r="E5" s="41"/>
-      <c r="F5" s="41"/>
+      <c r="B5" s="46" t="s">
+        <v>218</v>
+      </c>
+      <c r="C5" s="47"/>
+      <c r="D5" s="47"/>
+      <c r="E5" s="47"/>
+      <c r="F5" s="48"/>
       <c r="G5" s="30">
         <v>4</v>
       </c>
       <c r="H5" s="1"/>
     </row>
-    <row r="6" spans="1:8" ht="56.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" ht="56.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="29" t="s">
         <v>150</v>
       </c>
-      <c r="B6" s="41" t="s">
-        <v>200</v>
-      </c>
-      <c r="C6" s="41"/>
-      <c r="D6" s="41"/>
-      <c r="E6" s="41"/>
-      <c r="F6" s="41"/>
+      <c r="B6" s="46" t="s">
+        <v>187</v>
+      </c>
+      <c r="C6" s="47"/>
+      <c r="D6" s="47"/>
+      <c r="E6" s="47"/>
+      <c r="F6" s="48"/>
       <c r="G6" s="30">
         <v>7</v>
       </c>
       <c r="H6" s="1"/>
     </row>
-    <row r="7" spans="1:8" ht="56.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" ht="56.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="29" t="s">
         <v>151</v>
       </c>
-      <c r="B7" s="41" t="s">
-        <v>176</v>
-      </c>
-      <c r="C7" s="41"/>
-      <c r="D7" s="41"/>
-      <c r="E7" s="41"/>
-      <c r="F7" s="41"/>
+      <c r="B7" s="46" t="s">
+        <v>219</v>
+      </c>
+      <c r="C7" s="47"/>
+      <c r="D7" s="47"/>
+      <c r="E7" s="47"/>
+      <c r="F7" s="48"/>
       <c r="G7" s="30">
         <v>10</v>
       </c>
       <c r="H7" s="1"/>
     </row>
-    <row r="8" spans="1:8" ht="56.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" ht="56.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="29" t="s">
         <v>152</v>
       </c>
-      <c r="B8" s="41" t="s">
-        <v>175</v>
-      </c>
-      <c r="C8" s="41"/>
-      <c r="D8" s="41"/>
-      <c r="E8" s="41"/>
-      <c r="F8" s="41"/>
+      <c r="B8" s="46" t="s">
+        <v>220</v>
+      </c>
+      <c r="C8" s="47"/>
+      <c r="D8" s="47"/>
+      <c r="E8" s="47"/>
+      <c r="F8" s="48"/>
       <c r="G8" s="30">
         <v>13</v>
       </c>
       <c r="H8" s="1"/>
     </row>
-    <row r="9" spans="1:8" ht="56.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" ht="56.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="29" t="s">
         <v>153</v>
       </c>
-      <c r="B9" s="41" t="s">
-        <v>177</v>
-      </c>
-      <c r="C9" s="41"/>
-      <c r="D9" s="41"/>
-      <c r="E9" s="41"/>
-      <c r="F9" s="41"/>
+      <c r="B9" s="46" t="s">
+        <v>175</v>
+      </c>
+      <c r="C9" s="47"/>
+      <c r="D9" s="47"/>
+      <c r="E9" s="47"/>
+      <c r="F9" s="48"/>
       <c r="G9" s="30">
         <v>3</v>
       </c>
       <c r="H9" s="1"/>
     </row>
-    <row r="10" spans="1:8" ht="56.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" ht="56.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="29" t="s">
         <v>154</v>
       </c>
-      <c r="B10" s="41" t="s">
-        <v>178</v>
-      </c>
-      <c r="C10" s="41"/>
-      <c r="D10" s="41"/>
-      <c r="E10" s="41"/>
-      <c r="F10" s="41"/>
+      <c r="B10" s="46" t="s">
+        <v>221</v>
+      </c>
+      <c r="C10" s="47"/>
+      <c r="D10" s="47"/>
+      <c r="E10" s="47"/>
+      <c r="F10" s="48"/>
       <c r="G10" s="30">
         <v>3</v>
       </c>
       <c r="H10" s="1"/>
     </row>
-    <row r="11" spans="1:8" ht="56.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" ht="56.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="29" t="s">
         <v>155</v>
       </c>
-      <c r="B11" s="41" t="s">
-        <v>179</v>
-      </c>
-      <c r="C11" s="41"/>
-      <c r="D11" s="41"/>
-      <c r="E11" s="41"/>
-      <c r="F11" s="41"/>
+      <c r="B11" s="46" t="s">
+        <v>222</v>
+      </c>
+      <c r="C11" s="47"/>
+      <c r="D11" s="47"/>
+      <c r="E11" s="47"/>
+      <c r="F11" s="48"/>
       <c r="G11" s="30">
         <v>4</v>
       </c>
       <c r="H11" s="1"/>
     </row>
-    <row r="12" spans="1:8" ht="56.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" ht="56.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="29" t="s">
         <v>156</v>
       </c>
-      <c r="B12" s="41" t="s">
-        <v>180</v>
-      </c>
-      <c r="C12" s="41"/>
-      <c r="D12" s="41"/>
-      <c r="E12" s="41"/>
-      <c r="F12" s="41"/>
+      <c r="B12" s="46" t="s">
+        <v>200</v>
+      </c>
+      <c r="C12" s="47"/>
+      <c r="D12" s="47"/>
+      <c r="E12" s="47"/>
+      <c r="F12" s="48"/>
       <c r="G12" s="30">
         <v>9</v>
       </c>
       <c r="H12" s="1"/>
     </row>
-    <row r="13" spans="1:8" ht="56.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" ht="56.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="29" t="s">
         <v>157</v>
       </c>
-      <c r="B13" s="41" t="s">
-        <v>181</v>
-      </c>
-      <c r="C13" s="41"/>
-      <c r="D13" s="41"/>
-      <c r="E13" s="41"/>
-      <c r="F13" s="41"/>
+      <c r="B13" s="46" t="s">
+        <v>176</v>
+      </c>
+      <c r="C13" s="47"/>
+      <c r="D13" s="47"/>
+      <c r="E13" s="47"/>
+      <c r="F13" s="48"/>
       <c r="G13" s="30">
         <v>9</v>
       </c>
       <c r="H13" s="1"/>
     </row>
-    <row r="14" spans="1:8" ht="56.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" ht="56.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="29" t="s">
         <v>158</v>
       </c>
-      <c r="B14" s="41" t="s">
-        <v>182</v>
-      </c>
-      <c r="C14" s="41"/>
-      <c r="D14" s="41"/>
-      <c r="E14" s="41"/>
-      <c r="F14" s="41"/>
+      <c r="B14" s="46" t="s">
+        <v>223</v>
+      </c>
+      <c r="C14" s="47"/>
+      <c r="D14" s="47"/>
+      <c r="E14" s="47"/>
+      <c r="F14" s="48"/>
       <c r="G14" s="30">
         <v>5</v>
       </c>
       <c r="H14" s="1"/>
     </row>
-    <row r="15" spans="1:8" ht="56.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" ht="56.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="29" t="s">
         <v>159</v>
       </c>
-      <c r="B15" s="41" t="s">
-        <v>183</v>
-      </c>
-      <c r="C15" s="41"/>
-      <c r="D15" s="41"/>
-      <c r="E15" s="41"/>
-      <c r="F15" s="41"/>
+      <c r="B15" s="46" t="s">
+        <v>177</v>
+      </c>
+      <c r="C15" s="47"/>
+      <c r="D15" s="47"/>
+      <c r="E15" s="47"/>
+      <c r="F15" s="48"/>
       <c r="G15" s="30">
         <v>9</v>
       </c>
       <c r="H15" s="1"/>
     </row>
-    <row r="16" spans="1:8" ht="56.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" ht="56.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="29" t="s">
         <v>160</v>
       </c>
-      <c r="B16" s="41" t="s">
-        <v>184</v>
-      </c>
-      <c r="C16" s="41"/>
-      <c r="D16" s="41"/>
-      <c r="E16" s="41"/>
-      <c r="F16" s="41"/>
+      <c r="B16" s="46" t="s">
+        <v>178</v>
+      </c>
+      <c r="C16" s="47"/>
+      <c r="D16" s="47"/>
+      <c r="E16" s="47"/>
+      <c r="F16" s="48"/>
       <c r="G16" s="30">
         <v>9</v>
       </c>
       <c r="H16" s="1"/>
     </row>
-    <row r="17" spans="1:9" ht="56.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" ht="56.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="29" t="s">
         <v>161</v>
       </c>
-      <c r="B17" s="41" t="s">
-        <v>185</v>
-      </c>
-      <c r="C17" s="41"/>
-      <c r="D17" s="41"/>
-      <c r="E17" s="41"/>
-      <c r="F17" s="41"/>
+      <c r="B17" s="46" t="s">
+        <v>225</v>
+      </c>
+      <c r="C17" s="47"/>
+      <c r="D17" s="47"/>
+      <c r="E17" s="47"/>
+      <c r="F17" s="48"/>
       <c r="G17" s="30">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H17" s="1"/>
     </row>
-    <row r="18" spans="1:9" ht="56.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" ht="56.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="29" t="s">
         <v>162</v>
       </c>
-      <c r="B18" s="41" t="s">
-        <v>186</v>
-      </c>
-      <c r="C18" s="41"/>
-      <c r="D18" s="41"/>
-      <c r="E18" s="41"/>
-      <c r="F18" s="41"/>
+      <c r="B18" s="46" t="s">
+        <v>205</v>
+      </c>
+      <c r="C18" s="47"/>
+      <c r="D18" s="47"/>
+      <c r="E18" s="47"/>
+      <c r="F18" s="48"/>
       <c r="G18" s="30">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H18" s="1"/>
     </row>
-    <row r="19" spans="1:9" ht="56.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" ht="56.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="29" t="s">
         <v>163</v>
       </c>
-      <c r="B19" s="41" t="s">
-        <v>187</v>
-      </c>
-      <c r="C19" s="41"/>
-      <c r="D19" s="41"/>
-      <c r="E19" s="41"/>
-      <c r="F19" s="41"/>
+      <c r="B19" s="46" t="s">
+        <v>226</v>
+      </c>
+      <c r="C19" s="47"/>
+      <c r="D19" s="47"/>
+      <c r="E19" s="47"/>
+      <c r="F19" s="48"/>
       <c r="G19" s="30">
         <v>5</v>
       </c>
       <c r="H19" s="1"/>
     </row>
-    <row r="20" spans="1:9" ht="56.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" ht="56.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="29" t="s">
         <v>164</v>
       </c>
-      <c r="B20" s="41" t="s">
-        <v>188</v>
-      </c>
-      <c r="C20" s="41"/>
-      <c r="D20" s="41"/>
-      <c r="E20" s="41"/>
-      <c r="F20" s="41"/>
+      <c r="B20" s="46" t="s">
+        <v>227</v>
+      </c>
+      <c r="C20" s="47"/>
+      <c r="D20" s="47"/>
+      <c r="E20" s="47"/>
+      <c r="F20" s="48"/>
       <c r="G20" s="30">
         <v>4</v>
       </c>
       <c r="H20" s="1"/>
     </row>
-    <row r="21" spans="1:9" ht="56.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" ht="56.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="29" t="s">
         <v>165</v>
       </c>
-      <c r="B21" s="41" t="s">
-        <v>189</v>
-      </c>
-      <c r="C21" s="41"/>
-      <c r="D21" s="41"/>
-      <c r="E21" s="41"/>
-      <c r="F21" s="41"/>
+      <c r="B21" s="46" t="s">
+        <v>179</v>
+      </c>
+      <c r="C21" s="47"/>
+      <c r="D21" s="47"/>
+      <c r="E21" s="47"/>
+      <c r="F21" s="48"/>
       <c r="G21" s="30">
         <v>15</v>
       </c>
       <c r="H21" s="1"/>
     </row>
-    <row r="22" spans="1:9" ht="56.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" ht="56.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="29" t="s">
         <v>166</v>
       </c>
-      <c r="B22" s="41" t="s">
-        <v>190</v>
-      </c>
-      <c r="C22" s="41"/>
-      <c r="D22" s="41"/>
-      <c r="E22" s="41"/>
-      <c r="F22" s="41"/>
+      <c r="B22" s="46" t="s">
+        <v>228</v>
+      </c>
+      <c r="C22" s="47"/>
+      <c r="D22" s="47"/>
+      <c r="E22" s="47"/>
+      <c r="F22" s="48"/>
       <c r="G22" s="30">
         <v>9</v>
       </c>
       <c r="H22" s="1"/>
     </row>
-    <row r="23" spans="1:9" ht="56.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" ht="56.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="29" t="s">
         <v>167</v>
       </c>
-      <c r="B23" s="41" t="s">
-        <v>191</v>
-      </c>
-      <c r="C23" s="41"/>
-      <c r="D23" s="41"/>
-      <c r="E23" s="41"/>
-      <c r="F23" s="41"/>
+      <c r="B23" s="46" t="s">
+        <v>180</v>
+      </c>
+      <c r="C23" s="47"/>
+      <c r="D23" s="47"/>
+      <c r="E23" s="47"/>
+      <c r="F23" s="48"/>
       <c r="G23" s="30">
         <v>9</v>
       </c>
       <c r="H23" s="1"/>
     </row>
-    <row r="24" spans="1:9" ht="56.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" ht="56.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="29" t="s">
         <v>168</v>
       </c>
-      <c r="B24" s="41" t="s">
-        <v>192</v>
-      </c>
-      <c r="C24" s="41"/>
-      <c r="D24" s="41"/>
-      <c r="E24" s="41"/>
-      <c r="F24" s="41"/>
+      <c r="B24" s="46" t="s">
+        <v>181</v>
+      </c>
+      <c r="C24" s="47"/>
+      <c r="D24" s="47"/>
+      <c r="E24" s="47"/>
+      <c r="F24" s="48"/>
       <c r="G24" s="30">
         <v>14</v>
       </c>
       <c r="H24" s="1"/>
     </row>
-    <row r="25" spans="1:9" ht="56.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" ht="56.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="29" t="s">
         <v>169</v>
       </c>
-      <c r="B25" s="41" t="s">
-        <v>193</v>
-      </c>
-      <c r="C25" s="41"/>
-      <c r="D25" s="41"/>
-      <c r="E25" s="41"/>
-      <c r="F25" s="41"/>
+      <c r="B25" s="46" t="s">
+        <v>182</v>
+      </c>
+      <c r="C25" s="47"/>
+      <c r="D25" s="47"/>
+      <c r="E25" s="47"/>
+      <c r="F25" s="48"/>
       <c r="G25" s="30">
         <v>15</v>
       </c>
       <c r="H25" s="1"/>
     </row>
-    <row r="26" spans="1:9" ht="56.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" ht="56.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="29" t="s">
         <v>170</v>
       </c>
-      <c r="B26" s="41" t="s">
-        <v>194</v>
-      </c>
-      <c r="C26" s="41"/>
-      <c r="D26" s="41"/>
-      <c r="E26" s="41"/>
-      <c r="F26" s="41"/>
+      <c r="B26" s="46" t="s">
+        <v>183</v>
+      </c>
+      <c r="C26" s="47"/>
+      <c r="D26" s="47"/>
+      <c r="E26" s="47"/>
+      <c r="F26" s="48"/>
       <c r="G26" s="30">
         <v>16</v>
       </c>
       <c r="H26" s="1"/>
     </row>
-    <row r="27" spans="1:9" ht="56.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" ht="56.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="29" t="s">
         <v>171</v>
       </c>
-      <c r="B27" s="41" t="s">
-        <v>195</v>
-      </c>
-      <c r="C27" s="41"/>
-      <c r="D27" s="41"/>
-      <c r="E27" s="41"/>
-      <c r="F27" s="41"/>
+      <c r="B27" s="46" t="s">
+        <v>184</v>
+      </c>
+      <c r="C27" s="47"/>
+      <c r="D27" s="47"/>
+      <c r="E27" s="47"/>
+      <c r="F27" s="48"/>
       <c r="G27" s="30">
         <v>28</v>
       </c>
       <c r="H27" s="1"/>
     </row>
-    <row r="28" spans="1:9" ht="56.55" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:9" ht="56.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="33" t="s">
         <v>172</v>
       </c>
-      <c r="B28" s="42" t="s">
-        <v>196</v>
-      </c>
-      <c r="C28" s="42"/>
-      <c r="D28" s="42"/>
-      <c r="E28" s="42"/>
-      <c r="F28" s="42"/>
+      <c r="B28" s="60" t="s">
+        <v>185</v>
+      </c>
+      <c r="C28" s="61"/>
+      <c r="D28" s="61"/>
+      <c r="E28" s="61"/>
+      <c r="F28" s="62"/>
       <c r="G28" s="34">
         <v>25</v>
       </c>
       <c r="H28" s="1"/>
     </row>
-    <row r="29" spans="1:9" ht="56.55" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" ht="56.65" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A29" s="27"/>
-      <c r="B29" s="39" t="s">
-        <v>197</v>
-      </c>
-      <c r="C29" s="40"/>
-      <c r="D29" s="40"/>
-      <c r="E29" s="40"/>
-      <c r="F29" s="40"/>
+      <c r="B29" s="63" t="s">
+        <v>186</v>
+      </c>
+      <c r="C29" s="63"/>
+      <c r="D29" s="63"/>
+      <c r="E29" s="63"/>
+      <c r="F29" s="63"/>
       <c r="G29" s="28">
         <f>SUM(G3:G28)</f>
         <v>265</v>
       </c>
       <c r="H29" s="1"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G30" s="26"/>
       <c r="H30" s="13"/>
       <c r="I30" s="11"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G31" s="26"/>
       <c r="H31" s="13"/>
       <c r="I31" s="11"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G32" s="26"/>
       <c r="H32" s="13"/>
       <c r="I32" s="11"/>
     </row>
-    <row r="33" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="33" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G33" s="26"/>
       <c r="H33" s="13"/>
       <c r="I33" s="11"/>
     </row>
-    <row r="34" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="34" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G34" s="26"/>
       <c r="H34" s="13"/>
       <c r="I34" s="11"/>
     </row>
-    <row r="35" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="35" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G35" s="26"/>
       <c r="H35" s="13"/>
       <c r="I35" s="11"/>
     </row>
-    <row r="36" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="36" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G36" s="26"/>
       <c r="H36" s="13"/>
       <c r="J36" s="10"/>
     </row>
-    <row r="37" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="37" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G37" s="26"/>
       <c r="H37" s="13"/>
       <c r="I37" s="11"/>
       <c r="J37" s="10"/>
     </row>
-    <row r="38" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="38" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G38" s="26"/>
       <c r="H38" s="13"/>
       <c r="I38" s="11"/>
       <c r="J38" s="10"/>
     </row>
-    <row r="39" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="39" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G39" s="26"/>
       <c r="H39" s="13"/>
       <c r="I39" s="11"/>
       <c r="J39" s="10"/>
     </row>
-    <row r="40" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="40" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G40" s="26"/>
       <c r="H40" s="13"/>
       <c r="I40" s="11"/>
       <c r="J40" s="10"/>
     </row>
-    <row r="41" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="41" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G41" s="26"/>
       <c r="H41" s="13"/>
       <c r="I41" s="11"/>
       <c r="J41" s="10"/>
     </row>
-    <row r="42" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="42" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G42" s="26"/>
       <c r="H42" s="13"/>
       <c r="I42" s="11"/>
       <c r="J42" s="10"/>
     </row>
-    <row r="43" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="43" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G43" s="26"/>
       <c r="H43" s="24"/>
       <c r="I43" s="11"/>
       <c r="J43" s="10"/>
     </row>
-    <row r="44" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="44" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G44" s="26"/>
       <c r="H44" s="24"/>
       <c r="I44" s="11"/>
       <c r="J44" s="10"/>
     </row>
-    <row r="45" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="45" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G45" s="26"/>
       <c r="H45" s="13"/>
       <c r="I45" s="11"/>
       <c r="J45" s="10"/>
     </row>
-    <row r="46" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="46" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G46" s="26"/>
       <c r="H46" s="13"/>
       <c r="I46" s="11"/>
       <c r="J46" s="10"/>
     </row>
-    <row r="47" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="47" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G47" s="26"/>
       <c r="H47" s="13"/>
       <c r="I47" s="11"/>
       <c r="J47" s="10"/>
     </row>
-    <row r="48" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="48" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G48" s="26"/>
       <c r="H48" s="13"/>
       <c r="I48" s="11"/>
       <c r="J48" s="10"/>
     </row>
-    <row r="49" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="49" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G49" s="26"/>
       <c r="H49" s="13"/>
       <c r="I49" s="11"/>
       <c r="J49" s="10"/>
     </row>
-    <row r="50" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="50" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G50" s="26"/>
       <c r="H50" s="24"/>
       <c r="I50" s="11"/>
       <c r="J50" s="10"/>
     </row>
-    <row r="51" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="51" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G51" s="26"/>
       <c r="H51" s="24"/>
       <c r="J51" s="10"/>
     </row>
-    <row r="52" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="52" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G52" s="26"/>
       <c r="H52" s="24"/>
       <c r="J52" s="10"/>
     </row>
-    <row r="53" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="53" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G53" s="26"/>
       <c r="H53" s="24"/>
       <c r="J53" s="10"/>
     </row>
-    <row r="54" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="54" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G54" s="26"/>
       <c r="H54" s="24"/>
       <c r="J54" s="10"/>
     </row>
-    <row r="55" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="55" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G55" s="26"/>
       <c r="H55" s="20"/>
       <c r="I55" s="11"/>
       <c r="J55" s="10"/>
     </row>
-    <row r="56" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="56" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G56" s="26"/>
       <c r="I56" s="11"/>
       <c r="J56" s="10"/>
     </row>
-    <row r="57" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="57" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G57" s="26"/>
       <c r="J57" s="10"/>
     </row>
-    <row r="58" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="58" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G58" s="26"/>
       <c r="J58" s="10"/>
     </row>
-    <row r="59" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="59" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G59" s="26"/>
       <c r="H59" s="20"/>
       <c r="J59" s="10"/>
     </row>
-    <row r="60" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="60" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G60" s="26"/>
       <c r="J60" s="10"/>
     </row>
-    <row r="61" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="61" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G61" s="26"/>
       <c r="J61" s="10"/>
     </row>
-    <row r="62" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="62" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G62" s="26"/>
       <c r="H62" s="20"/>
       <c r="J62" s="10"/>
     </row>
-    <row r="63" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="63" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G63" s="26"/>
       <c r="J63" s="10"/>
     </row>
-    <row r="64" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="64" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G64" s="26"/>
       <c r="H64" s="20"/>
       <c r="J64" s="10"/>
     </row>
-    <row r="65" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="65" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G65" s="26"/>
       <c r="H65" s="20"/>
       <c r="J65" s="10"/>
     </row>
-    <row r="66" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="66" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G66" s="26"/>
       <c r="J66" s="10"/>
     </row>
-    <row r="67" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="67" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G67" s="26"/>
       <c r="J67" s="10"/>
     </row>
-    <row r="68" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="68" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G68" s="26"/>
       <c r="J68" s="10"/>
     </row>
-    <row r="69" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="69" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G69" s="26"/>
       <c r="J69" s="10"/>
     </row>
-    <row r="70" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="70" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G70" s="26"/>
       <c r="H70" s="20"/>
       <c r="I70" s="37"/>
       <c r="J70" s="38"/>
     </row>
-    <row r="71" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="71" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G71" s="26"/>
       <c r="I71" s="37"/>
       <c r="J71" s="38"/>
     </row>
-    <row r="72" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="72" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G72" s="26"/>
       <c r="H72" s="20"/>
       <c r="J72" s="21"/>
     </row>
-    <row r="73" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="73" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G73" s="26"/>
       <c r="H73" s="20"/>
       <c r="J73" s="21"/>
     </row>
-    <row r="74" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="74" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G74" s="26"/>
       <c r="H74" s="20"/>
       <c r="J74" s="21"/>
     </row>
-    <row r="75" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="75" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G75" s="26"/>
       <c r="H75" s="20"/>
       <c r="I75" s="11"/>
       <c r="J75" s="21"/>
     </row>
-    <row r="76" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="76" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G76" s="26"/>
       <c r="J76" s="21"/>
     </row>
-    <row r="77" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="77" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G77" s="26"/>
       <c r="H77" s="20"/>
       <c r="J77" s="21"/>
     </row>
-    <row r="78" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="78" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G78" s="26"/>
       <c r="J78" s="21"/>
     </row>
-    <row r="79" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="79" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G79" s="26"/>
       <c r="J79" s="21"/>
     </row>
-    <row r="80" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="80" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G80" s="26"/>
       <c r="J80" s="21"/>
     </row>
-    <row r="81" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="81" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G81" s="26"/>
       <c r="H81" s="20"/>
       <c r="J81" s="21"/>
     </row>
-    <row r="82" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="82" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G82" s="26"/>
       <c r="H82" s="20"/>
       <c r="J82" s="21"/>
     </row>
-    <row r="83" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="83" spans="7:10" x14ac:dyDescent="0.25">
       <c r="J83" s="21"/>
     </row>
-    <row r="84" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="84" spans="7:10" x14ac:dyDescent="0.25">
       <c r="H84" s="20"/>
       <c r="J84" s="21"/>
     </row>
-    <row r="85" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="85" spans="7:10" x14ac:dyDescent="0.25">
       <c r="J85" s="21"/>
     </row>
-    <row r="86" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="86" spans="7:10" x14ac:dyDescent="0.25">
       <c r="H86" s="20"/>
       <c r="J86" s="21"/>
     </row>
-    <row r="87" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="87" spans="7:10" x14ac:dyDescent="0.25">
       <c r="H87" s="20"/>
       <c r="J87" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="32">
-    <mergeCell ref="G1:G2"/>
-    <mergeCell ref="B3:F3"/>
-    <mergeCell ref="B4:F4"/>
-    <mergeCell ref="B5:F5"/>
-    <mergeCell ref="B6:F6"/>
-    <mergeCell ref="B7:F7"/>
-    <mergeCell ref="B8:F8"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:F2"/>
-    <mergeCell ref="B9:F9"/>
-    <mergeCell ref="B10:F10"/>
-    <mergeCell ref="B13:F13"/>
-    <mergeCell ref="B11:F11"/>
-    <mergeCell ref="B12:F12"/>
-    <mergeCell ref="B14:F14"/>
-    <mergeCell ref="B15:F15"/>
-    <mergeCell ref="B16:F16"/>
-    <mergeCell ref="B18:F18"/>
-    <mergeCell ref="B17:F17"/>
-    <mergeCell ref="B19:F19"/>
-    <mergeCell ref="B20:F20"/>
-    <mergeCell ref="B21:F21"/>
-    <mergeCell ref="B22:F22"/>
-    <mergeCell ref="B23:F23"/>
-    <mergeCell ref="I70:I71"/>
     <mergeCell ref="J70:J71"/>
     <mergeCell ref="B29:F29"/>
     <mergeCell ref="B24:F24"/>
@@ -3866,6 +4051,31 @@
     <mergeCell ref="B26:F26"/>
     <mergeCell ref="B27:F27"/>
     <mergeCell ref="B28:F28"/>
+    <mergeCell ref="B20:F20"/>
+    <mergeCell ref="B21:F21"/>
+    <mergeCell ref="B22:F22"/>
+    <mergeCell ref="B23:F23"/>
+    <mergeCell ref="I70:I71"/>
+    <mergeCell ref="B15:F15"/>
+    <mergeCell ref="B16:F16"/>
+    <mergeCell ref="B18:F18"/>
+    <mergeCell ref="B17:F17"/>
+    <mergeCell ref="B19:F19"/>
+    <mergeCell ref="B10:F10"/>
+    <mergeCell ref="B13:F13"/>
+    <mergeCell ref="B11:F11"/>
+    <mergeCell ref="B12:F12"/>
+    <mergeCell ref="B14:F14"/>
+    <mergeCell ref="B7:F7"/>
+    <mergeCell ref="B8:F8"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:F2"/>
+    <mergeCell ref="B9:F9"/>
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="B4:F4"/>
+    <mergeCell ref="B5:F5"/>
+    <mergeCell ref="B6:F6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3879,335 +4089,335 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J89"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageLayout" zoomScale="90" zoomScaleNormal="100" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="E66" sqref="E66"/>
+    <sheetView showGridLines="0" view="pageLayout" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.109375" customWidth="1"/>
+    <col min="1" max="1" width="14.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="43" t="s">
-        <v>201</v>
-      </c>
-      <c r="B1" s="43" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="39" t="s">
+        <v>188</v>
+      </c>
+      <c r="B1" s="39" t="s">
         <v>146</v>
       </c>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
-      <c r="G1" s="43" t="s">
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39" t="s">
         <v>147</v>
       </c>
       <c r="H1" s="1"/>
     </row>
-    <row r="2" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="44"/>
-      <c r="B2" s="44"/>
-      <c r="C2" s="44"/>
-      <c r="D2" s="44"/>
-      <c r="E2" s="44"/>
-      <c r="F2" s="44"/>
-      <c r="G2" s="44"/>
+    <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="40"/>
+      <c r="B2" s="40"/>
+      <c r="C2" s="40"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="40"/>
+      <c r="G2" s="40"/>
       <c r="H2" s="1"/>
     </row>
-    <row r="3" spans="1:8" ht="56.55" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="56.65" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="31" t="s">
         <v>173</v>
       </c>
-      <c r="B3" s="45" t="s">
+      <c r="B3" s="41" t="s">
         <v>174</v>
       </c>
-      <c r="C3" s="45"/>
-      <c r="D3" s="45"/>
-      <c r="E3" s="45"/>
-      <c r="F3" s="45"/>
+      <c r="C3" s="41"/>
+      <c r="D3" s="41"/>
+      <c r="E3" s="41"/>
+      <c r="F3" s="41"/>
       <c r="G3" s="32">
         <v>5</v>
       </c>
       <c r="H3" s="1"/>
     </row>
-    <row r="4" spans="1:8" ht="56.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="56.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="29" t="s">
         <v>148</v>
       </c>
-      <c r="B4" s="41" t="s">
-        <v>204</v>
-      </c>
-      <c r="C4" s="41"/>
-      <c r="D4" s="41"/>
-      <c r="E4" s="41"/>
-      <c r="F4" s="41"/>
+      <c r="B4" s="42" t="s">
+        <v>191</v>
+      </c>
+      <c r="C4" s="42"/>
+      <c r="D4" s="42"/>
+      <c r="E4" s="42"/>
+      <c r="F4" s="42"/>
       <c r="G4" s="30">
         <v>16</v>
       </c>
       <c r="H4" s="1"/>
     </row>
-    <row r="5" spans="1:8" ht="56.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" ht="56.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="29" t="s">
-        <v>202</v>
+        <v>189</v>
       </c>
       <c r="B5" s="46" t="s">
-        <v>203</v>
+        <v>190</v>
       </c>
       <c r="C5" s="47"/>
       <c r="D5" s="47"/>
       <c r="E5" s="47"/>
       <c r="F5" s="48"/>
       <c r="G5" s="30" t="s">
-        <v>205</v>
+        <v>192</v>
       </c>
       <c r="H5" s="1"/>
     </row>
-    <row r="6" spans="1:8" ht="56.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" ht="56.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="29" t="s">
         <v>149</v>
       </c>
-      <c r="B6" s="41" t="s">
-        <v>206</v>
-      </c>
-      <c r="C6" s="41"/>
-      <c r="D6" s="41"/>
-      <c r="E6" s="41"/>
-      <c r="F6" s="41"/>
+      <c r="B6" s="42" t="s">
+        <v>193</v>
+      </c>
+      <c r="C6" s="42"/>
+      <c r="D6" s="42"/>
+      <c r="E6" s="42"/>
+      <c r="F6" s="42"/>
       <c r="G6" s="30">
         <v>4</v>
       </c>
       <c r="H6" s="1"/>
     </row>
-    <row r="7" spans="1:8" ht="56.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" ht="56.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="29" t="s">
         <v>150</v>
       </c>
-      <c r="B7" s="41" t="s">
-        <v>207</v>
-      </c>
-      <c r="C7" s="41"/>
-      <c r="D7" s="41"/>
-      <c r="E7" s="41"/>
-      <c r="F7" s="41"/>
+      <c r="B7" s="42" t="s">
+        <v>194</v>
+      </c>
+      <c r="C7" s="42"/>
+      <c r="D7" s="42"/>
+      <c r="E7" s="42"/>
+      <c r="F7" s="42"/>
       <c r="G7" s="30">
         <v>7</v>
       </c>
       <c r="H7" s="1"/>
     </row>
-    <row r="8" spans="1:8" ht="56.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" ht="56.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="29" t="s">
         <v>151</v>
       </c>
-      <c r="B8" s="41" t="s">
-        <v>208</v>
-      </c>
-      <c r="C8" s="41"/>
-      <c r="D8" s="41"/>
-      <c r="E8" s="41"/>
-      <c r="F8" s="41"/>
+      <c r="B8" s="42" t="s">
+        <v>195</v>
+      </c>
+      <c r="C8" s="42"/>
+      <c r="D8" s="42"/>
+      <c r="E8" s="42"/>
+      <c r="F8" s="42"/>
       <c r="G8" s="30">
         <v>6</v>
       </c>
       <c r="H8" s="1"/>
     </row>
-    <row r="9" spans="1:8" ht="56.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" ht="56.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="29" t="s">
         <v>152</v>
       </c>
-      <c r="B9" s="41" t="s">
-        <v>209</v>
-      </c>
-      <c r="C9" s="41"/>
-      <c r="D9" s="41"/>
-      <c r="E9" s="41"/>
-      <c r="F9" s="41"/>
+      <c r="B9" s="42" t="s">
+        <v>196</v>
+      </c>
+      <c r="C9" s="42"/>
+      <c r="D9" s="42"/>
+      <c r="E9" s="42"/>
+      <c r="F9" s="42"/>
       <c r="G9" s="30">
         <v>6</v>
       </c>
       <c r="H9" s="1"/>
     </row>
-    <row r="10" spans="1:8" ht="56.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" ht="56.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="29" t="s">
         <v>153</v>
       </c>
-      <c r="B10" s="41" t="s">
-        <v>210</v>
-      </c>
-      <c r="C10" s="41"/>
-      <c r="D10" s="41"/>
-      <c r="E10" s="41"/>
-      <c r="F10" s="41"/>
+      <c r="B10" s="42" t="s">
+        <v>197</v>
+      </c>
+      <c r="C10" s="42"/>
+      <c r="D10" s="42"/>
+      <c r="E10" s="42"/>
+      <c r="F10" s="42"/>
       <c r="G10" s="30">
         <v>7</v>
       </c>
       <c r="H10" s="1"/>
     </row>
-    <row r="11" spans="1:8" ht="56.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" ht="56.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="29" t="s">
         <v>154</v>
       </c>
-      <c r="B11" s="41" t="s">
-        <v>211</v>
-      </c>
-      <c r="C11" s="41"/>
-      <c r="D11" s="41"/>
-      <c r="E11" s="41"/>
-      <c r="F11" s="41"/>
+      <c r="B11" s="42" t="s">
+        <v>198</v>
+      </c>
+      <c r="C11" s="42"/>
+      <c r="D11" s="42"/>
+      <c r="E11" s="42"/>
+      <c r="F11" s="42"/>
       <c r="G11" s="30">
         <v>1</v>
       </c>
       <c r="H11" s="1"/>
     </row>
-    <row r="12" spans="1:8" ht="56.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" ht="56.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="29" t="s">
         <v>155</v>
       </c>
-      <c r="B12" s="41" t="s">
-        <v>212</v>
-      </c>
-      <c r="C12" s="41"/>
-      <c r="D12" s="41"/>
-      <c r="E12" s="41"/>
-      <c r="F12" s="41"/>
+      <c r="B12" s="42" t="s">
+        <v>199</v>
+      </c>
+      <c r="C12" s="42"/>
+      <c r="D12" s="42"/>
+      <c r="E12" s="42"/>
+      <c r="F12" s="42"/>
       <c r="G12" s="30">
         <v>9</v>
       </c>
       <c r="H12" s="1"/>
     </row>
-    <row r="13" spans="1:8" ht="56.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" ht="56.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="29" t="s">
         <v>156</v>
       </c>
-      <c r="B13" s="41" t="s">
-        <v>213</v>
-      </c>
-      <c r="C13" s="41"/>
-      <c r="D13" s="41"/>
-      <c r="E13" s="41"/>
-      <c r="F13" s="41"/>
+      <c r="B13" s="42" t="s">
+        <v>200</v>
+      </c>
+      <c r="C13" s="42"/>
+      <c r="D13" s="42"/>
+      <c r="E13" s="42"/>
+      <c r="F13" s="42"/>
       <c r="G13" s="30">
         <v>9</v>
       </c>
       <c r="H13" s="1"/>
     </row>
-    <row r="14" spans="1:8" ht="56.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" ht="56.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="29" t="s">
         <v>157</v>
       </c>
-      <c r="B14" s="41" t="s">
-        <v>214</v>
-      </c>
-      <c r="C14" s="41"/>
-      <c r="D14" s="41"/>
-      <c r="E14" s="41"/>
-      <c r="F14" s="41"/>
+      <c r="B14" s="42" t="s">
+        <v>201</v>
+      </c>
+      <c r="C14" s="42"/>
+      <c r="D14" s="42"/>
+      <c r="E14" s="42"/>
+      <c r="F14" s="42"/>
       <c r="G14" s="30">
         <v>9</v>
       </c>
       <c r="H14" s="1"/>
     </row>
-    <row r="15" spans="1:8" ht="56.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" ht="56.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="29" t="s">
         <v>158</v>
       </c>
-      <c r="B15" s="41" t="s">
-        <v>215</v>
-      </c>
-      <c r="C15" s="41"/>
-      <c r="D15" s="41"/>
-      <c r="E15" s="41"/>
-      <c r="F15" s="41"/>
+      <c r="B15" s="42" t="s">
+        <v>202</v>
+      </c>
+      <c r="C15" s="42"/>
+      <c r="D15" s="42"/>
+      <c r="E15" s="42"/>
+      <c r="F15" s="42"/>
       <c r="G15" s="30">
         <v>9</v>
       </c>
       <c r="H15" s="1"/>
     </row>
-    <row r="16" spans="1:8" ht="56.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" ht="56.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="29" t="s">
         <v>159</v>
       </c>
-      <c r="B16" s="41" t="s">
-        <v>216</v>
-      </c>
-      <c r="C16" s="41"/>
-      <c r="D16" s="41"/>
-      <c r="E16" s="41"/>
-      <c r="F16" s="41"/>
+      <c r="B16" s="42" t="s">
+        <v>203</v>
+      </c>
+      <c r="C16" s="42"/>
+      <c r="D16" s="42"/>
+      <c r="E16" s="42"/>
+      <c r="F16" s="42"/>
       <c r="G16" s="30">
         <v>9</v>
       </c>
       <c r="H16" s="1"/>
     </row>
-    <row r="17" spans="1:9" ht="56.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" ht="56.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="29" t="s">
         <v>160</v>
       </c>
-      <c r="B17" s="41" t="s">
-        <v>217</v>
-      </c>
-      <c r="C17" s="41"/>
-      <c r="D17" s="41"/>
-      <c r="E17" s="41"/>
-      <c r="F17" s="41"/>
+      <c r="B17" s="42" t="s">
+        <v>204</v>
+      </c>
+      <c r="C17" s="42"/>
+      <c r="D17" s="42"/>
+      <c r="E17" s="42"/>
+      <c r="F17" s="42"/>
       <c r="G17" s="30">
         <v>9</v>
       </c>
       <c r="H17" s="1"/>
     </row>
-    <row r="18" spans="1:9" ht="56.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" ht="56.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="29" t="s">
         <v>161</v>
       </c>
-      <c r="B18" s="41" t="s">
-        <v>218</v>
-      </c>
-      <c r="C18" s="41"/>
-      <c r="D18" s="41"/>
-      <c r="E18" s="41"/>
-      <c r="F18" s="41"/>
+      <c r="B18" s="42" t="s">
+        <v>224</v>
+      </c>
+      <c r="C18" s="42"/>
+      <c r="D18" s="42"/>
+      <c r="E18" s="42"/>
+      <c r="F18" s="42"/>
       <c r="G18" s="30">
         <v>8</v>
       </c>
       <c r="H18" s="1"/>
     </row>
-    <row r="19" spans="1:9" ht="56.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" ht="56.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="29" t="s">
         <v>162</v>
       </c>
-      <c r="B19" s="41" t="s">
-        <v>219</v>
-      </c>
-      <c r="C19" s="41"/>
-      <c r="D19" s="41"/>
-      <c r="E19" s="41"/>
-      <c r="F19" s="41"/>
+      <c r="B19" s="42" t="s">
+        <v>205</v>
+      </c>
+      <c r="C19" s="42"/>
+      <c r="D19" s="42"/>
+      <c r="E19" s="42"/>
+      <c r="F19" s="42"/>
       <c r="G19" s="30">
         <v>5</v>
       </c>
       <c r="H19" s="1"/>
     </row>
-    <row r="20" spans="1:9" ht="56.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" ht="56.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="29" t="s">
         <v>163</v>
       </c>
-      <c r="B20" s="41" t="s">
-        <v>220</v>
-      </c>
-      <c r="C20" s="41"/>
-      <c r="D20" s="41"/>
-      <c r="E20" s="41"/>
-      <c r="F20" s="41"/>
+      <c r="B20" s="42" t="s">
+        <v>206</v>
+      </c>
+      <c r="C20" s="42"/>
+      <c r="D20" s="42"/>
+      <c r="E20" s="42"/>
+      <c r="F20" s="42"/>
       <c r="G20" s="30">
         <v>6</v>
       </c>
       <c r="H20" s="1"/>
     </row>
-    <row r="21" spans="1:9" ht="56.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" ht="56.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="29" t="s">
-        <v>221</v>
+        <v>207</v>
       </c>
       <c r="B21" s="46" t="s">
-        <v>222</v>
+        <v>208</v>
       </c>
       <c r="C21" s="47"/>
       <c r="D21" s="47"/>
@@ -4218,454 +4428,472 @@
       </c>
       <c r="H21" s="1"/>
     </row>
-    <row r="22" spans="1:9" ht="56.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" ht="56.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="29" t="s">
         <v>164</v>
       </c>
-      <c r="B22" s="41" t="s">
-        <v>223</v>
-      </c>
-      <c r="C22" s="41"/>
-      <c r="D22" s="41"/>
-      <c r="E22" s="41"/>
-      <c r="F22" s="41"/>
+      <c r="B22" s="42" t="s">
+        <v>209</v>
+      </c>
+      <c r="C22" s="42"/>
+      <c r="D22" s="42"/>
+      <c r="E22" s="42"/>
+      <c r="F22" s="42"/>
       <c r="G22" s="30">
         <v>4</v>
       </c>
       <c r="H22" s="1"/>
     </row>
-    <row r="23" spans="1:9" ht="56.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" ht="56.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="29" t="s">
         <v>165</v>
       </c>
-      <c r="B23" s="41" t="s">
-        <v>224</v>
-      </c>
-      <c r="C23" s="41"/>
-      <c r="D23" s="41"/>
-      <c r="E23" s="41"/>
-      <c r="F23" s="41"/>
+      <c r="B23" s="42" t="s">
+        <v>210</v>
+      </c>
+      <c r="C23" s="42"/>
+      <c r="D23" s="42"/>
+      <c r="E23" s="42"/>
+      <c r="F23" s="42"/>
       <c r="G23" s="30">
         <v>7</v>
       </c>
       <c r="H23" s="1"/>
     </row>
-    <row r="24" spans="1:9" ht="56.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" ht="56.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="29" t="s">
         <v>166</v>
       </c>
-      <c r="B24" s="41" t="s">
-        <v>225</v>
-      </c>
-      <c r="C24" s="41"/>
-      <c r="D24" s="41"/>
-      <c r="E24" s="41"/>
-      <c r="F24" s="41"/>
+      <c r="B24" s="42" t="s">
+        <v>211</v>
+      </c>
+      <c r="C24" s="42"/>
+      <c r="D24" s="42"/>
+      <c r="E24" s="42"/>
+      <c r="F24" s="42"/>
       <c r="G24" s="30">
         <v>9</v>
       </c>
       <c r="H24" s="1"/>
     </row>
-    <row r="25" spans="1:9" ht="56.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" ht="56.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="29" t="s">
         <v>167</v>
       </c>
-      <c r="B25" s="41" t="s">
-        <v>226</v>
-      </c>
-      <c r="C25" s="41"/>
-      <c r="D25" s="41"/>
-      <c r="E25" s="41"/>
-      <c r="F25" s="41"/>
+      <c r="B25" s="42" t="s">
+        <v>212</v>
+      </c>
+      <c r="C25" s="42"/>
+      <c r="D25" s="42"/>
+      <c r="E25" s="42"/>
+      <c r="F25" s="42"/>
       <c r="G25" s="30">
         <v>10</v>
       </c>
       <c r="H25" s="1"/>
     </row>
-    <row r="26" spans="1:9" ht="56.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" ht="56.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="29" t="s">
         <v>168</v>
       </c>
-      <c r="B26" s="41" t="s">
-        <v>227</v>
-      </c>
-      <c r="C26" s="41"/>
-      <c r="D26" s="41"/>
-      <c r="E26" s="41"/>
-      <c r="F26" s="41"/>
+      <c r="B26" s="42" t="s">
+        <v>213</v>
+      </c>
+      <c r="C26" s="42"/>
+      <c r="D26" s="42"/>
+      <c r="E26" s="42"/>
+      <c r="F26" s="42"/>
       <c r="G26" s="30">
         <v>9</v>
       </c>
       <c r="H26" s="1"/>
     </row>
-    <row r="27" spans="1:9" ht="56.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" ht="56.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="29" t="s">
         <v>169</v>
       </c>
-      <c r="B27" s="41" t="s">
-        <v>228</v>
-      </c>
-      <c r="C27" s="41"/>
-      <c r="D27" s="41"/>
-      <c r="E27" s="41"/>
-      <c r="F27" s="41"/>
+      <c r="B27" s="42" t="s">
+        <v>214</v>
+      </c>
+      <c r="C27" s="42"/>
+      <c r="D27" s="42"/>
+      <c r="E27" s="42"/>
+      <c r="F27" s="42"/>
       <c r="G27" s="30">
         <v>15</v>
       </c>
       <c r="H27" s="1"/>
     </row>
-    <row r="28" spans="1:9" ht="56.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" ht="56.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="29" t="s">
         <v>170</v>
       </c>
-      <c r="B28" s="41" t="s">
-        <v>230</v>
-      </c>
-      <c r="C28" s="41"/>
-      <c r="D28" s="41"/>
-      <c r="E28" s="41"/>
-      <c r="F28" s="41"/>
+      <c r="B28" s="42" t="s">
+        <v>216</v>
+      </c>
+      <c r="C28" s="42"/>
+      <c r="D28" s="42"/>
+      <c r="E28" s="42"/>
+      <c r="F28" s="42"/>
       <c r="G28" s="30">
         <v>5</v>
       </c>
       <c r="H28" s="1"/>
     </row>
-    <row r="29" spans="1:9" ht="56.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" ht="56.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="29" t="s">
         <v>171</v>
       </c>
-      <c r="B29" s="41" t="s">
-        <v>224</v>
-      </c>
-      <c r="C29" s="41"/>
-      <c r="D29" s="41"/>
-      <c r="E29" s="41"/>
-      <c r="F29" s="41"/>
+      <c r="B29" s="42" t="s">
+        <v>210</v>
+      </c>
+      <c r="C29" s="42"/>
+      <c r="D29" s="42"/>
+      <c r="E29" s="42"/>
+      <c r="F29" s="42"/>
       <c r="G29" s="30">
         <v>7</v>
       </c>
       <c r="H29" s="1"/>
     </row>
-    <row r="30" spans="1:9" ht="56.55" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:9" ht="56.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="33" t="s">
         <v>172</v>
       </c>
-      <c r="B30" s="42" t="s">
-        <v>229</v>
-      </c>
-      <c r="C30" s="42"/>
-      <c r="D30" s="42"/>
-      <c r="E30" s="42"/>
-      <c r="F30" s="42"/>
+      <c r="B30" s="45" t="s">
+        <v>215</v>
+      </c>
+      <c r="C30" s="45"/>
+      <c r="D30" s="45"/>
+      <c r="E30" s="45"/>
+      <c r="F30" s="45"/>
       <c r="G30" s="34">
         <v>8</v>
       </c>
       <c r="H30" s="1"/>
     </row>
-    <row r="31" spans="1:9" ht="56.55" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" ht="56.65" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A31" s="27"/>
-      <c r="B31" s="39" t="s">
-        <v>197</v>
-      </c>
-      <c r="C31" s="40"/>
-      <c r="D31" s="40"/>
-      <c r="E31" s="40"/>
-      <c r="F31" s="40"/>
+      <c r="B31" s="43" t="s">
+        <v>186</v>
+      </c>
+      <c r="C31" s="44"/>
+      <c r="D31" s="44"/>
+      <c r="E31" s="44"/>
+      <c r="F31" s="44"/>
       <c r="G31" s="28">
         <f>SUM(G3:G30)</f>
         <v>203</v>
       </c>
       <c r="H31" s="1"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G32" s="26"/>
       <c r="H32" s="13"/>
       <c r="I32" s="11"/>
     </row>
-    <row r="33" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="33" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G33" s="26"/>
       <c r="H33" s="13"/>
       <c r="I33" s="11"/>
     </row>
-    <row r="34" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="34" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G34" s="26"/>
       <c r="H34" s="13"/>
       <c r="I34" s="11"/>
     </row>
-    <row r="35" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="35" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G35" s="26"/>
       <c r="H35" s="13"/>
       <c r="I35" s="11"/>
     </row>
-    <row r="36" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="36" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G36" s="26"/>
       <c r="H36" s="13"/>
       <c r="I36" s="11"/>
     </row>
-    <row r="37" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="37" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G37" s="26"/>
       <c r="H37" s="13"/>
       <c r="I37" s="11"/>
     </row>
-    <row r="38" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="38" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G38" s="26"/>
       <c r="H38" s="13"/>
       <c r="J38" s="10"/>
     </row>
-    <row r="39" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="39" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G39" s="26"/>
       <c r="H39" s="13"/>
       <c r="I39" s="11"/>
       <c r="J39" s="10"/>
     </row>
-    <row r="40" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="40" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G40" s="26"/>
       <c r="H40" s="13"/>
       <c r="I40" s="11"/>
       <c r="J40" s="10"/>
     </row>
-    <row r="41" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="41" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G41" s="26"/>
       <c r="H41" s="13"/>
       <c r="I41" s="11"/>
       <c r="J41" s="10"/>
     </row>
-    <row r="42" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="42" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G42" s="26"/>
       <c r="H42" s="13"/>
       <c r="I42" s="11"/>
       <c r="J42" s="10"/>
     </row>
-    <row r="43" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="43" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G43" s="26"/>
       <c r="H43" s="13"/>
       <c r="I43" s="11"/>
       <c r="J43" s="10"/>
     </row>
-    <row r="44" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="44" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G44" s="26"/>
       <c r="H44" s="13"/>
       <c r="I44" s="11"/>
       <c r="J44" s="10"/>
     </row>
-    <row r="45" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="45" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G45" s="26"/>
       <c r="H45" s="25"/>
       <c r="I45" s="11"/>
       <c r="J45" s="10"/>
     </row>
-    <row r="46" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="46" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G46" s="26"/>
       <c r="H46" s="25"/>
       <c r="I46" s="11"/>
       <c r="J46" s="10"/>
     </row>
-    <row r="47" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="47" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G47" s="26"/>
       <c r="H47" s="13"/>
       <c r="I47" s="11"/>
       <c r="J47" s="10"/>
     </row>
-    <row r="48" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="48" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G48" s="26"/>
       <c r="H48" s="13"/>
       <c r="I48" s="11"/>
       <c r="J48" s="10"/>
     </row>
-    <row r="49" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="49" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G49" s="26"/>
       <c r="H49" s="13"/>
       <c r="I49" s="11"/>
       <c r="J49" s="10"/>
     </row>
-    <row r="50" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="50" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G50" s="26"/>
       <c r="H50" s="13"/>
       <c r="I50" s="11"/>
       <c r="J50" s="10"/>
     </row>
-    <row r="51" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="51" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G51" s="26"/>
       <c r="H51" s="13"/>
       <c r="I51" s="11"/>
       <c r="J51" s="10"/>
     </row>
-    <row r="52" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="52" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G52" s="26"/>
       <c r="H52" s="25"/>
       <c r="I52" s="11"/>
       <c r="J52" s="10"/>
     </row>
-    <row r="53" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="53" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G53" s="26"/>
       <c r="H53" s="25"/>
       <c r="J53" s="10"/>
     </row>
-    <row r="54" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="54" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G54" s="26"/>
       <c r="H54" s="25"/>
       <c r="J54" s="10"/>
     </row>
-    <row r="55" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="55" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G55" s="26"/>
       <c r="H55" s="25"/>
       <c r="J55" s="10"/>
     </row>
-    <row r="56" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="56" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G56" s="26"/>
       <c r="H56" s="25"/>
       <c r="J56" s="10"/>
     </row>
-    <row r="57" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="57" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G57" s="26"/>
       <c r="H57" s="20"/>
       <c r="I57" s="11"/>
       <c r="J57" s="10"/>
     </row>
-    <row r="58" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="58" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G58" s="26"/>
       <c r="I58" s="11"/>
       <c r="J58" s="10"/>
     </row>
-    <row r="59" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="59" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G59" s="26"/>
       <c r="J59" s="10"/>
     </row>
-    <row r="60" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="60" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G60" s="26"/>
       <c r="J60" s="10"/>
     </row>
-    <row r="61" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="61" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G61" s="26"/>
       <c r="H61" s="20"/>
       <c r="J61" s="10"/>
     </row>
-    <row r="62" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="62" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G62" s="26"/>
       <c r="J62" s="10"/>
     </row>
-    <row r="63" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="63" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G63" s="26"/>
       <c r="J63" s="10"/>
     </row>
-    <row r="64" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="64" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G64" s="26"/>
       <c r="H64" s="20"/>
       <c r="J64" s="10"/>
     </row>
-    <row r="65" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="65" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G65" s="26"/>
       <c r="J65" s="10"/>
     </row>
-    <row r="66" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="66" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G66" s="26"/>
       <c r="H66" s="20"/>
       <c r="J66" s="10"/>
     </row>
-    <row r="67" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="67" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G67" s="26"/>
       <c r="H67" s="20"/>
       <c r="J67" s="10"/>
     </row>
-    <row r="68" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="68" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G68" s="26"/>
       <c r="J68" s="10"/>
     </row>
-    <row r="69" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="69" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G69" s="26"/>
       <c r="J69" s="10"/>
     </row>
-    <row r="70" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="70" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G70" s="26"/>
       <c r="J70" s="10"/>
     </row>
-    <row r="71" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="71" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G71" s="26"/>
       <c r="J71" s="10"/>
     </row>
-    <row r="72" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="72" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G72" s="26"/>
       <c r="H72" s="20"/>
       <c r="I72" s="37"/>
       <c r="J72" s="38"/>
     </row>
-    <row r="73" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="73" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G73" s="26"/>
       <c r="I73" s="37"/>
       <c r="J73" s="38"/>
     </row>
-    <row r="74" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="74" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G74" s="26"/>
       <c r="H74" s="20"/>
       <c r="J74" s="21"/>
     </row>
-    <row r="75" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="75" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G75" s="26"/>
       <c r="H75" s="20"/>
       <c r="J75" s="21"/>
     </row>
-    <row r="76" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="76" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G76" s="26"/>
       <c r="H76" s="20"/>
       <c r="J76" s="21"/>
     </row>
-    <row r="77" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="77" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G77" s="26"/>
       <c r="H77" s="20"/>
       <c r="I77" s="11"/>
       <c r="J77" s="21"/>
     </row>
-    <row r="78" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="78" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G78" s="26"/>
       <c r="J78" s="21"/>
     </row>
-    <row r="79" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="79" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G79" s="26"/>
       <c r="H79" s="20"/>
       <c r="J79" s="21"/>
     </row>
-    <row r="80" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="80" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G80" s="26"/>
       <c r="J80" s="21"/>
     </row>
-    <row r="81" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="81" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G81" s="26"/>
       <c r="J81" s="21"/>
     </row>
-    <row r="82" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="82" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G82" s="26"/>
       <c r="J82" s="21"/>
     </row>
-    <row r="83" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="83" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G83" s="26"/>
       <c r="H83" s="20"/>
       <c r="J83" s="21"/>
     </row>
-    <row r="84" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="84" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G84" s="26"/>
       <c r="H84" s="20"/>
       <c r="J84" s="21"/>
     </row>
-    <row r="85" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="85" spans="7:10" x14ac:dyDescent="0.25">
       <c r="J85" s="21"/>
     </row>
-    <row r="86" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="86" spans="7:10" x14ac:dyDescent="0.25">
       <c r="H86" s="20"/>
       <c r="J86" s="21"/>
     </row>
-    <row r="87" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="87" spans="7:10" x14ac:dyDescent="0.25">
       <c r="J87" s="21"/>
     </row>
-    <row r="88" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="88" spans="7:10" x14ac:dyDescent="0.25">
       <c r="H88" s="20"/>
       <c r="J88" s="21"/>
     </row>
-    <row r="89" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="89" spans="7:10" x14ac:dyDescent="0.25">
       <c r="H89" s="20"/>
       <c r="J89" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="34">
+    <mergeCell ref="B6:F6"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:F2"/>
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="B4:F4"/>
+    <mergeCell ref="B18:F18"/>
+    <mergeCell ref="B7:F7"/>
+    <mergeCell ref="B8:F8"/>
+    <mergeCell ref="B9:F9"/>
+    <mergeCell ref="B10:F10"/>
+    <mergeCell ref="B11:F11"/>
+    <mergeCell ref="B12:F12"/>
+    <mergeCell ref="B13:F13"/>
+    <mergeCell ref="B14:F14"/>
+    <mergeCell ref="B15:F15"/>
+    <mergeCell ref="B16:F16"/>
+    <mergeCell ref="B17:F17"/>
     <mergeCell ref="I72:I73"/>
     <mergeCell ref="J72:J73"/>
     <mergeCell ref="B5:F5"/>
@@ -4682,24 +4910,6 @@
     <mergeCell ref="B23:F23"/>
     <mergeCell ref="B24:F24"/>
     <mergeCell ref="B25:F25"/>
-    <mergeCell ref="B13:F13"/>
-    <mergeCell ref="B14:F14"/>
-    <mergeCell ref="B15:F15"/>
-    <mergeCell ref="B16:F16"/>
-    <mergeCell ref="B17:F17"/>
-    <mergeCell ref="B18:F18"/>
-    <mergeCell ref="B7:F7"/>
-    <mergeCell ref="B8:F8"/>
-    <mergeCell ref="B9:F9"/>
-    <mergeCell ref="B10:F10"/>
-    <mergeCell ref="B11:F11"/>
-    <mergeCell ref="B12:F12"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:F2"/>
-    <mergeCell ref="G1:G2"/>
-    <mergeCell ref="B3:F3"/>
-    <mergeCell ref="B4:F4"/>
-    <mergeCell ref="B6:F6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>